<commit_message>
I have updated skyscanner flight search2
</commit_message>
<xml_diff>
--- a/Skyscanner_Test_cases_Search_Flights.xlsx
+++ b/Skyscanner_Test_cases_Search_Flights.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-465" windowWidth="20730" windowHeight="11760" tabRatio="500" firstSheet="7" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="-465" windowWidth="20730" windowHeight="11760" tabRatio="500" firstSheet="10" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,8 +15,11 @@
     <sheet name="Thomas cook" sheetId="6" r:id="rId6"/>
     <sheet name="Thetrainline" sheetId="7" r:id="rId7"/>
     <sheet name="skyscanner Flight Search" sheetId="8" r:id="rId8"/>
-    <sheet name="Skyscanner Hotel Search1" sheetId="9" r:id="rId9"/>
-    <sheet name="Skyscanner CarHire Search" sheetId="10" r:id="rId10"/>
+    <sheet name="Skyscanner CarHire Search" sheetId="10" r:id="rId9"/>
+    <sheet name="Skyscanner Hotel Search" sheetId="9" r:id="rId10"/>
+    <sheet name="Skyscanner Flight search2" sheetId="11" r:id="rId11"/>
+    <sheet name="Skyscanner Hotel Search2" sheetId="12" r:id="rId12"/>
+    <sheet name="Skyscanner Carhire Search2" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="396">
   <si>
     <t>Test ID</t>
   </si>
@@ -804,20 +807,7 @@
     <t>"Flights is a default search page of the website</t>
   </si>
   <si>
-    <t>1) Navigete to the Website www.skyscanner.co.uk
-2) Add "Southampton" in "From" Search space
-3)Add "Manchester" in "To" Search space</t>
-  </si>
-  <si>
-    <t>1) Select "One way" journerney
-2) Press "Search Flights"</t>
-  </si>
-  <si>
     <t>As a user I found fight schedulels from "flybe"</t>
-  </si>
-  <si>
-    <t>1) Select "Return" journerney
-2) Press "Search Flights"</t>
   </si>
   <si>
     <t xml:space="preserve">As a user I shold expect flights schedules from "flybe" </t>
@@ -835,10 +825,6 @@
   </si>
   <si>
     <t>Select "Multi-city"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) Navigete to the Website www.skyscanner.co.uk
-</t>
   </si>
   <si>
     <t>As a user I should expect
@@ -1121,6 +1107,309 @@
   </si>
   <si>
     <t>As a user I found search results in the next page</t>
+  </si>
+  <si>
+    <t>Verify that the user can search for one way flight in the website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Navigete to the Website www.skyscanner.co.uk
+</t>
+  </si>
+  <si>
+    <t>1) Add "Southampton" in "From" Search space
+2)Add "Manchester" in "To" Search space
+3) Select "One way" journerney
+4) Press "Search Flights"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Navigete to the Website www.skyscanner.co.uk
+</t>
+  </si>
+  <si>
+    <t>Verify that the user can search return flight in the website</t>
+  </si>
+  <si>
+    <t>1) Add "Southampton" in "From" Search space
+2)Add "Manchester" in "To" Search space
+3) Select "Return" journerney
+4) Press "Search Flights"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigete to the Website www.skyscanner.co.uk
+</t>
+  </si>
+  <si>
+    <t>Verify that the user can search for "Multi flights" in the website</t>
+  </si>
+  <si>
+    <t>Verify that the user can search for Direct flights in the website</t>
+  </si>
+  <si>
+    <t>Verify that the user can be moved to the partner websites for flight booking successfully</t>
+  </si>
+  <si>
+    <t>Verify that the User can use search  on the website</t>
+  </si>
+  <si>
+    <t>Verify that the user can search flights with valid name</t>
+  </si>
+  <si>
+    <t>Verify that user can search flights using capital alphabets</t>
+  </si>
+  <si>
+    <t>Verify that the user can search flights by using only first alphabet of the name</t>
+  </si>
+  <si>
+    <t>Verify that the user can search flights with invalid dates</t>
+  </si>
+  <si>
+    <t>Verify that the user can saerch for return flights</t>
+  </si>
+  <si>
+    <t>verify that the user can search flights for multiple destinations</t>
+  </si>
+  <si>
+    <t>Verify that the user can search for direct flight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the user can find full detials of the flights  </t>
+  </si>
+  <si>
+    <t>Verify that the user can search hotel by a hotel name</t>
+  </si>
+  <si>
+    <t>Verify that the user can search hotel by city name</t>
+  </si>
+  <si>
+    <t>Verify that the user can search a hotel by country name</t>
+  </si>
+  <si>
+    <t>Verify that the user can search a hotel by valid name</t>
+  </si>
+  <si>
+    <t>Verify that the user can serch a hotel by using invalid name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the user can search a hotel by using only capital alphabets </t>
+  </si>
+  <si>
+    <t>Verify that the user can search a hotel by using only small alphabets</t>
+  </si>
+  <si>
+    <t>Verify that the user can search hotels by using valid date</t>
+  </si>
+  <si>
+    <t>Verify that the user can search a hotels by using invalid date</t>
+  </si>
+  <si>
+    <t>Verify that the user can search a hotels by using future check-in date for over one and half year</t>
+  </si>
+  <si>
+    <t>Verify that the using can search hotles by using a past date check-in</t>
+  </si>
+  <si>
+    <t>Verify that the user can search hotles by using guests over 10 guests in number</t>
+  </si>
+  <si>
+    <t>Verify that the user can search hotels with room more than 5 rooms avaialable</t>
+  </si>
+  <si>
+    <t>Verify that the user can search hotels in two cities in one search</t>
+  </si>
+  <si>
+    <t>Verify that user can search hotels by using search terms</t>
+  </si>
+  <si>
+    <t>Verify that the user can search a car hire by using city name</t>
+  </si>
+  <si>
+    <t>Verify that the user can search a car hire by using country name</t>
+  </si>
+  <si>
+    <t>Verify that user can search a car hire by using wrong city name</t>
+  </si>
+  <si>
+    <t>Verify that the user can search a car hire by using only capital alphabets</t>
+  </si>
+  <si>
+    <t>Verify that the user can search car hire by using numbers</t>
+  </si>
+  <si>
+    <t>Verify that user can search car hire by using wrong date</t>
+  </si>
+  <si>
+    <t>Verify that the user can search car hire by using pickup date for over 2 years in future</t>
+  </si>
+  <si>
+    <t>Verify that the user can search car hire by using a return address in the same city</t>
+  </si>
+  <si>
+    <t>verify that the usr can search car hire by using a return address in different country</t>
+  </si>
+  <si>
+    <t>Verify that the user can search a car hire if his age is less than 18</t>
+  </si>
+  <si>
+    <t>verify that the user can search a car hire if his age is over 75</t>
+  </si>
+  <si>
+    <t>Verify that the user can Search a car hire with the pick up time 1 am</t>
+  </si>
+  <si>
+    <t>Verify that user can search airport transers with a valid date</t>
+  </si>
+  <si>
+    <t>Verify that the user can search air port transers with an invalid date</t>
+  </si>
+  <si>
+    <t>Verify that the user can search airport trasfers for more than 24 passengers</t>
+  </si>
+  <si>
+    <t>1)Enter "Southampton" in the search box
+2) Press "Searh flights" without changing any other detials</t>
+  </si>
+  <si>
+    <t>Verify that the user can search flights with invalid name</t>
+  </si>
+  <si>
+    <t>As a user I expect that the search results will open in next page with the option to select the destination</t>
+  </si>
+  <si>
+    <t>As a user I found that the search results opened in next page with the option to select the destination</t>
+  </si>
+  <si>
+    <t>As a user I expect that "Southampton" should appear in suggestions</t>
+  </si>
+  <si>
+    <t>As a user I found that the website did not suggest or pick "Southampton" as a city</t>
+  </si>
+  <si>
+    <t>As a user I found that the website suggested "Southampton" as a city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user I expect that the website should provied all the names contain "s" </t>
+  </si>
+  <si>
+    <t>As a user I found that the website provied all the names contain "s"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter "S" in the search box
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter "Sou" in the search box
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter "Soton" in the search box
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter "SOUTHAMPTON" in the search box 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user I found that "Southampton" appeared in search suggestions </t>
+  </si>
+  <si>
+    <t>Verify that user can search flights by using only small alphabets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter "southampton" in the search box </t>
+  </si>
+  <si>
+    <t>verify that the user can search flights by mixing numbers</t>
+  </si>
+  <si>
+    <t>Enter "S0uthampton" in the search box</t>
+  </si>
+  <si>
+    <t>As a user I expect that the website should suggest names by using first alphabet of the search name</t>
+  </si>
+  <si>
+    <t>Verify that the user can search flights by using three alphabets of the name</t>
+  </si>
+  <si>
+    <t>As a user I found that the website suggested names by using first alphabet of the search name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the user can search for future flights with two  years future dates for </t>
+  </si>
+  <si>
+    <t>Enter "3/09/2018" in Depart date box</t>
+  </si>
+  <si>
+    <t>As auser I expect that the website should not let me enter past date</t>
+  </si>
+  <si>
+    <t>As a user I found that the website did not let me enter past date</t>
+  </si>
+  <si>
+    <t>Enter "04/09/2020" in Depart date box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user I found that the website did not allow date late than one and  half year in future </t>
+  </si>
+  <si>
+    <t>As a user I expect that the website should not allow dates late than one and  half year in future</t>
+  </si>
+  <si>
+    <t>Verify that the user can search one way flights</t>
+  </si>
+  <si>
+    <t>As a user I shold expect one way flight schedules from "Southampton to Manchester"</t>
+  </si>
+  <si>
+    <t>As a user I found one way flight schedules from "Southampton to Manchester"</t>
+  </si>
+  <si>
+    <t>As a user I found return  flight schedules between "Southampton To Manchester and Manchester To Southampton"</t>
+  </si>
+  <si>
+    <t>1Select "Multi-city"
+2) Add "Southampton" in "From" Search space
+3)Add "Manchester" in "To" Search space
+4) add "Manchester" in third entry point in "From"
+5) Add "Glasgow" in fourth entry point in "To"
+6) select "12/09/2018" as expected journey date
+7) Press "Search Flights"</t>
+  </si>
+  <si>
+    <t>As a user I should expect return  flight schedules between "Southampton To Manchester and Manchester To Southampton"</t>
+  </si>
+  <si>
+    <t>As a user I should expect flight schedules from "Southampton To Manchester" and "Manchester To Glasgow"</t>
+  </si>
+  <si>
+    <t>As a user I found flight schedules from "Southampton To Manchester" and "Manchester To Glasgow"</t>
+  </si>
+  <si>
+    <t>As a user I should expect Direct flight schedules from "London To Munich" with no "stops"</t>
+  </si>
+  <si>
+    <t>1) Add "London" in "From" Search space
+2)Add "Munich" in "To" Search space
+3) Select Direct Flights Only
+4) Press "Search Flights"</t>
+  </si>
+  <si>
+    <t>As a user I found direct flights Shedules from "London to Munich" with no "stops"</t>
+  </si>
+  <si>
+    <t>Verify that the user can find Flight detials in the website</t>
+  </si>
+  <si>
+    <t>1) Add "London Heathrow" in "From" Search space
+2)Add "Munich" in "To" Search space
+3) Select Direct Flights Only 
+4) Press "Search Flights"
+5) Press "Select" 1 deal of "Lufthansa airline"</t>
+  </si>
+  <si>
+    <t>As a user I expect flight schedule to open in next page with details</t>
+  </si>
+  <si>
+    <t>As a user I found flight schedule to open in next page with details</t>
   </si>
 </sst>
 </file>
@@ -1407,7 +1696,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1941,21 +2230,366 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:W11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <pane xSplit="8" topLeftCell="W1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="5.625" customWidth="1"/>
-    <col min="2" max="2" width="17.25" customWidth="1"/>
-    <col min="3" max="3" width="23.5" customWidth="1"/>
-    <col min="4" max="4" width="33.375" customWidth="1"/>
-    <col min="5" max="5" width="29.75" customWidth="1"/>
-    <col min="6" max="6" width="22.5" customWidth="1"/>
+    <col min="1" max="1" width="6.875" customWidth="1"/>
+    <col min="2" max="2" width="22.25" customWidth="1"/>
+    <col min="3" max="3" width="24.625" customWidth="1"/>
+    <col min="4" max="4" width="22.5" customWidth="1"/>
+    <col min="5" max="5" width="25.375" customWidth="1"/>
+    <col min="6" max="6" width="23.5" customWidth="1"/>
+    <col min="8" max="8" width="10.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23">
+      <c r="A1" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="W1" s="9" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="78.75">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="78.75">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="W3" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="94.5">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="W4" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="94.5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="W5" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="110.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="W6" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="94.5">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="W7" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="110.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="W8" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="157.5">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="W9" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="94.5">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="W10" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="63">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="W11" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="6.75" customWidth="1"/>
+    <col min="2" max="2" width="23.25" customWidth="1"/>
+    <col min="3" max="3" width="24.875" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="23.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1987,27 +2621,27 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="78.75">
+    <row r="2" spans="1:9" ht="63.75" customHeight="1">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>288</v>
+        <v>315</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>289</v>
+        <v>222</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>290</v>
+        <v>353</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>294</v>
+        <v>355</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>295</v>
+        <v>356</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>18</v>
+        <v>193</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>14</v>
@@ -2018,25 +2652,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>288</v>
+        <v>354</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>291</v>
+        <v>222</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>292</v>
+        <v>364</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>14</v>
+        <v>358</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="63">
@@ -2044,22 +2675,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>288</v>
+        <v>372</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>293</v>
+        <v>222</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>296</v>
+        <v>363</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>299</v>
+        <v>357</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>193</v>
+        <v>359</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>14</v>
@@ -2070,51 +2698,629 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>288</v>
+        <v>317</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>293</v>
+        <v>222</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>301</v>
+        <v>362</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>302</v>
+        <v>360</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>303</v>
+        <v>361</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>245</v>
+        <v>193</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="94.5">
+    <row r="6" spans="1:9" ht="47.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>288</v>
+        <v>316</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>304</v>
+        <v>222</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>305</v>
+        <v>365</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>306</v>
+        <v>357</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>307</v>
+        <v>366</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>193</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="47.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="63">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="47.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="63">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="104.25" customHeight="1">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="94.5">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="189">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="117" customHeight="1">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="126">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="189">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="6.375" customWidth="1"/>
+    <col min="2" max="2" width="19.875" customWidth="1"/>
+    <col min="3" max="3" width="22.125" customWidth="1"/>
+    <col min="4" max="4" width="28.875" customWidth="1"/>
+    <col min="5" max="5" width="33.25" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="47.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="47.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="47.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="47.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="47.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="63">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="63">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="47.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="47.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="63">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="78.75">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="63">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="63">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="63">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="47.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="6.125" customWidth="1"/>
+    <col min="2" max="2" width="21.375" customWidth="1"/>
+    <col min="3" max="3" width="27.75" customWidth="1"/>
+    <col min="4" max="4" width="31.125" customWidth="1"/>
+    <col min="5" max="5" width="30.875" customWidth="1"/>
+    <col min="6" max="6" width="23.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="47.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="47.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="47.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="63">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="47.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="47.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="63">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="63">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="63">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="47.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="47.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="47.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="47.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="47.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="63">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -3476,9 +4682,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3551,19 +4757,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>221</v>
+        <v>304</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>193</v>
@@ -3577,19 +4783,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>221</v>
+        <v>308</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>225</v>
+        <v>305</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>231</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>193</v>
@@ -3603,19 +4809,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>221</v>
+        <v>311</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>234</v>
+        <v>310</v>
       </c>
       <c r="D5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>193</v>
@@ -3629,19 +4835,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>221</v>
+        <v>311</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>193</v>
@@ -3661,13 +4867,13 @@
         <v>222</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>193</v>
@@ -3681,22 +4887,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>221</v>
+        <v>312</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>222</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>14</v>
@@ -3707,19 +4913,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>221</v>
+        <v>312</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>222</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>193</v>
@@ -3733,19 +4939,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>221</v>
+        <v>392</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>222</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>193</v>
@@ -3759,19 +4965,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>221</v>
+        <v>313</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>222</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>193</v>
@@ -3787,27 +4993,26 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <pane xSplit="8" topLeftCell="W1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="6.875" customWidth="1"/>
-    <col min="2" max="2" width="22.25" customWidth="1"/>
-    <col min="3" max="3" width="24.625" customWidth="1"/>
-    <col min="4" max="4" width="22.5" customWidth="1"/>
-    <col min="5" max="5" width="25.375" customWidth="1"/>
-    <col min="6" max="6" width="23.5" customWidth="1"/>
-    <col min="8" max="8" width="10.375" customWidth="1"/>
+    <col min="1" max="1" width="5.625" customWidth="1"/>
+    <col min="2" max="2" width="17.25" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="33.375" customWidth="1"/>
+    <col min="5" max="5" width="29.75" customWidth="1"/>
+    <col min="6" max="6" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:9">
       <c r="A1" s="5" t="s">
-        <v>147</v>
+        <v>220</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>145</v>
@@ -3833,299 +5038,138 @@
       <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="W1" s="9" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" ht="78.75">
+    </row>
+    <row r="2" spans="1:9" ht="78.75">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>256</v>
+        <v>284</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>222</v>
+        <v>285</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>262</v>
+        <v>290</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>263</v>
+        <v>291</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>193</v>
+        <v>18</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="W2" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" ht="78.75">
+    </row>
+    <row r="3" spans="1:9" ht="63">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>256</v>
+        <v>284</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>258</v>
+        <v>287</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>259</v>
+        <v>288</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>261</v>
+        <v>293</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>260</v>
+        <v>294</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>193</v>
+        <v>18</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="W3" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" ht="94.5">
+    </row>
+    <row r="4" spans="1:9" ht="63">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>256</v>
+        <v>284</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>258</v>
+        <v>289</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>266</v>
+        <v>296</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>18</v>
+        <v>193</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="W4" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="94.5">
+    </row>
+    <row r="5" spans="1:9" ht="63">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>256</v>
+        <v>284</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>258</v>
+        <v>289</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>272</v>
+        <v>297</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>269</v>
+        <v>298</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>268</v>
+        <v>299</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>18</v>
+        <v>241</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="W5" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" ht="110.25">
+    </row>
+    <row r="6" spans="1:9" ht="94.5">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>256</v>
+        <v>284</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>258</v>
+        <v>300</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>265</v>
+        <v>301</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>270</v>
+        <v>302</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>271</v>
+        <v>303</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>18</v>
+        <v>193</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="W6" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="94.5">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="W7" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" ht="110.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="W8" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" ht="157.5">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="W9" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" ht="94.5">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="W10" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" ht="63">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="W11" s="9" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
i have updated the file
</commit_message>
<xml_diff>
--- a/Skyscanner_Test_cases_Search_Flights.xlsx
+++ b/Skyscanner_Test_cases_Search_Flights.xlsx
@@ -1468,9 +1468,6 @@
     <t>Verify that the user can serch journey by using special characters</t>
   </si>
   <si>
-    <t>Verify that the user can search for a return journey in future after eight month from the present date</t>
-  </si>
-  <si>
     <t>Verify that user can search for a journey on 29/02/2020 in leap year</t>
   </si>
   <si>
@@ -1647,6 +1644,9 @@
   </si>
   <si>
     <t>As a user I found that the website did not let me search for the journey</t>
+  </si>
+  <si>
+    <t>Verify that the user can search for a  journey in future after eight month from the present date</t>
   </si>
 </sst>
 </file>
@@ -1936,7 +1936,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3691,7 +3691,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3740,16 +3740,16 @@
         <v>410</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>422</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>423</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>27</v>
@@ -3763,16 +3763,16 @@
         <v>411</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>425</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>426</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>14</v>
@@ -3783,19 +3783,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>412</v>
+        <v>464</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>427</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>428</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>27</v>
@@ -3806,7 +3806,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="78.75">
@@ -3814,19 +3814,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>432</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>433</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>27</v>
@@ -3837,19 +3837,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>435</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>436</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>27</v>
@@ -3860,19 +3860,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>458</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>459</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>14</v>
@@ -3883,19 +3883,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>463</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>464</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>14</v>
@@ -3906,19 +3906,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>439</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>440</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>27</v>
@@ -3929,19 +3929,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>442</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>443</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>14</v>
@@ -3952,19 +3952,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>445</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>446</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>14</v>
@@ -3975,19 +3975,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="I13" s="9"/>
     </row>
@@ -3996,19 +3996,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>451</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>452</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>14</v>
@@ -4019,19 +4019,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>454</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>455</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>14</v>
@@ -4042,7 +4042,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added for thomas cook
</commit_message>
<xml_diff>
--- a/Skyscanner_Test_cases_Search_Flights.xlsx
+++ b/Skyscanner_Test_cases_Search_Flights.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-465" windowWidth="20730" windowHeight="11760" tabRatio="500" firstSheet="12" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="-465" windowWidth="20730" windowHeight="11760" tabRatio="500" firstSheet="12" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Skyscanner Carhire Search2" sheetId="13" r:id="rId13"/>
     <sheet name="Trainline Search test" sheetId="14" r:id="rId14"/>
     <sheet name="Thomascook Search Test" sheetId="15" r:id="rId15"/>
+    <sheet name="Sheet3" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="481">
   <si>
     <t>Test ID</t>
   </si>
@@ -1694,6 +1695,10 @@
   </si>
   <si>
     <t>As a user I found that the word "Southampton" appeared in flying from</t>
+  </si>
+  <si>
+    <t>1) Enter "southampton" search terms for find flying from
+2) Press enter</t>
   </si>
 </sst>
 </file>
@@ -1983,7 +1988,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4101,9 +4106,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -4167,12 +4172,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="47.25">
+    <row r="3" spans="1:9" ht="63">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>466</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="63">
@@ -4245,6 +4265,51 @@
       </c>
       <c r="B12" s="1" t="s">
         <v>476</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>